<commit_message>
FileTabRibbonEnableDisable feature and FileTabRibbonIsDisplayed feature included. Test fail - unable to interrogate "File Tab" Excel sheet updated.
</commit_message>
<xml_diff>
--- a/Documents/REquirement Estimations.xlsx
+++ b/Documents/REquirement Estimations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SAMAutomation\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B5855F-7825-4A80-80D2-C6945C7B28DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D37CBF-5ED4-49A4-BC48-F20C87EAE63D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="10596" windowHeight="7548" xr2:uid="{11A85534-C6CC-46D9-9A7F-116C480C3734}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1818" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1831" uniqueCount="633">
   <si>
     <t>New</t>
   </si>
@@ -2258,7 +2258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -2418,68 +2418,8 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -2493,15 +2433,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2522,6 +2453,93 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2839,8 +2857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11CE17E-1AC3-466A-A104-5C7FF12BF975}">
   <dimension ref="A3:D1664"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B47" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A706" workbookViewId="0">
+      <selection activeCell="D264" sqref="D264:D265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2873,7 +2891,7 @@
       <c r="A7" s="53">
         <v>1</v>
       </c>
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="79" t="s">
         <v>562</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -2883,25 +2901,25 @@
     </row>
     <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="53"/>
-      <c r="B8" s="76"/>
+      <c r="B8" s="80"/>
       <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="68" t="s">
+        <v>630</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="53"/>
-      <c r="B9" s="76"/>
+      <c r="B9" s="80"/>
       <c r="C9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="74" t="s">
-        <v>628</v>
-      </c>
+      <c r="D9" s="76"/>
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="53"/>
-      <c r="B10" s="76"/>
+      <c r="B10" s="80"/>
       <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
@@ -2909,7 +2927,7 @@
     </row>
     <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="53"/>
-      <c r="B11" s="76"/>
+      <c r="B11" s="80"/>
       <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
@@ -2917,7 +2935,7 @@
     </row>
     <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="53"/>
-      <c r="B12" s="76"/>
+      <c r="B12" s="80"/>
       <c r="C12" s="3" t="s">
         <v>5</v>
       </c>
@@ -2925,7 +2943,7 @@
     </row>
     <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="53"/>
-      <c r="B13" s="76"/>
+      <c r="B13" s="80"/>
       <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
@@ -2933,7 +2951,7 @@
     </row>
     <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="53"/>
-      <c r="B14" s="77"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="3" t="s">
         <v>7</v>
       </c>
@@ -2943,7 +2961,7 @@
       <c r="A15" s="53">
         <v>2</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="79" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -2953,7 +2971,7 @@
     </row>
     <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="53"/>
-      <c r="B16" s="76"/>
+      <c r="B16" s="80"/>
       <c r="C16" s="3" t="s">
         <v>1</v>
       </c>
@@ -2961,25 +2979,25 @@
     </row>
     <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="53"/>
-      <c r="B17" s="76"/>
+      <c r="B17" s="80"/>
       <c r="C17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="4"/>
+      <c r="D17" s="68" t="s">
+        <v>630</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="53"/>
-      <c r="B18" s="76"/>
+      <c r="B18" s="80"/>
       <c r="C18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="74" t="s">
-        <v>628</v>
-      </c>
+      <c r="D18" s="76"/>
     </row>
     <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="53"/>
-      <c r="B19" s="76"/>
+      <c r="B19" s="80"/>
       <c r="C19" s="3" t="s">
         <v>4</v>
       </c>
@@ -2987,7 +3005,7 @@
     </row>
     <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="53"/>
-      <c r="B20" s="76"/>
+      <c r="B20" s="80"/>
       <c r="C20" s="3" t="s">
         <v>5</v>
       </c>
@@ -2995,7 +3013,7 @@
     </row>
     <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="53"/>
-      <c r="B21" s="76"/>
+      <c r="B21" s="80"/>
       <c r="C21" s="3" t="s">
         <v>6</v>
       </c>
@@ -3003,7 +3021,7 @@
     </row>
     <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="53"/>
-      <c r="B22" s="77"/>
+      <c r="B22" s="81"/>
       <c r="C22" s="3" t="s">
         <v>7</v>
       </c>
@@ -3013,7 +3031,7 @@
       <c r="A23" s="53">
         <v>3</v>
       </c>
-      <c r="B23" s="75" t="s">
+      <c r="B23" s="79" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -3023,15 +3041,17 @@
     </row>
     <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="53"/>
-      <c r="B24" s="76"/>
+      <c r="B24" s="80"/>
       <c r="C24" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="4"/>
+      <c r="D24" s="68" t="s">
+        <v>630</v>
+      </c>
     </row>
     <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="53"/>
-      <c r="B25" s="76"/>
+      <c r="B25" s="80"/>
       <c r="C25" s="3" t="s">
         <v>2</v>
       </c>
@@ -3039,7 +3059,7 @@
     </row>
     <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="53"/>
-      <c r="B26" s="76"/>
+      <c r="B26" s="80"/>
       <c r="C26" s="3" t="s">
         <v>3</v>
       </c>
@@ -3047,17 +3067,15 @@
     </row>
     <row r="27" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="53"/>
-      <c r="B27" s="76"/>
+      <c r="B27" s="80"/>
       <c r="C27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="74" t="s">
-        <v>628</v>
-      </c>
+      <c r="D27" s="76"/>
     </row>
     <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="53"/>
-      <c r="B28" s="76"/>
+      <c r="B28" s="80"/>
       <c r="C28" s="3" t="s">
         <v>5</v>
       </c>
@@ -3065,7 +3083,7 @@
     </row>
     <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="53"/>
-      <c r="B29" s="76"/>
+      <c r="B29" s="80"/>
       <c r="C29" s="3" t="s">
         <v>6</v>
       </c>
@@ -3073,7 +3091,7 @@
     </row>
     <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="53"/>
-      <c r="B30" s="77"/>
+      <c r="B30" s="81"/>
       <c r="C30" s="3" t="s">
         <v>7</v>
       </c>
@@ -3083,7 +3101,7 @@
       <c r="A31" s="53">
         <v>4</v>
       </c>
-      <c r="B31" s="75" t="s">
+      <c r="B31" s="82" t="s">
         <v>10</v>
       </c>
       <c r="C31" s="6" t="s">
@@ -3093,25 +3111,23 @@
     </row>
     <row r="32" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="53"/>
-      <c r="B32" s="76"/>
+      <c r="B32" s="83"/>
       <c r="C32" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="74" t="s">
-        <v>628</v>
-      </c>
+      <c r="D32" s="76"/>
     </row>
     <row r="33" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="53"/>
-      <c r="B33" s="76"/>
+      <c r="B33" s="83"/>
       <c r="C33" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="99"/>
+      <c r="D33" s="76"/>
     </row>
     <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="53"/>
-      <c r="B34" s="76"/>
+      <c r="B34" s="83"/>
       <c r="C34" s="7" t="s">
         <v>14</v>
       </c>
@@ -3119,7 +3135,7 @@
     </row>
     <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="53"/>
-      <c r="B35" s="76"/>
+      <c r="B35" s="83"/>
       <c r="C35" s="6" t="s">
         <v>15</v>
       </c>
@@ -3127,7 +3143,7 @@
     </row>
     <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="53"/>
-      <c r="B36" s="76"/>
+      <c r="B36" s="83"/>
       <c r="C36" s="6" t="s">
         <v>16</v>
       </c>
@@ -3135,7 +3151,7 @@
     </row>
     <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="53"/>
-      <c r="B37" s="76"/>
+      <c r="B37" s="83"/>
       <c r="C37" s="6" t="s">
         <v>17</v>
       </c>
@@ -3143,23 +3159,25 @@
     </row>
     <row r="38" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="53"/>
-      <c r="B38" s="76"/>
+      <c r="B38" s="83"/>
       <c r="C38" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D38" s="99"/>
-    </row>
-    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D38" s="76"/>
+    </row>
+    <row r="39" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="53"/>
-      <c r="B39" s="76"/>
+      <c r="B39" s="83"/>
       <c r="C39" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="4"/>
+      <c r="D39" s="63" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="53"/>
-      <c r="B40" s="76"/>
+      <c r="B40" s="83"/>
       <c r="C40" s="6" t="s">
         <v>20</v>
       </c>
@@ -3167,7 +3185,7 @@
     </row>
     <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="53"/>
-      <c r="B41" s="76"/>
+      <c r="B41" s="83"/>
       <c r="C41" s="6" t="s">
         <v>21</v>
       </c>
@@ -3175,7 +3193,7 @@
     </row>
     <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="53"/>
-      <c r="B42" s="76"/>
+      <c r="B42" s="83"/>
       <c r="C42" s="6" t="s">
         <v>22</v>
       </c>
@@ -3183,7 +3201,7 @@
     </row>
     <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="53"/>
-      <c r="B43" s="76"/>
+      <c r="B43" s="83"/>
       <c r="C43" s="6" t="s">
         <v>23</v>
       </c>
@@ -3191,7 +3209,7 @@
     </row>
     <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="53"/>
-      <c r="B44" s="76"/>
+      <c r="B44" s="83"/>
       <c r="C44" s="6" t="s">
         <v>24</v>
       </c>
@@ -3199,7 +3217,7 @@
     </row>
     <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="53"/>
-      <c r="B45" s="76"/>
+      <c r="B45" s="83"/>
       <c r="C45" s="6" t="s">
         <v>25</v>
       </c>
@@ -3207,7 +3225,7 @@
     </row>
     <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="53"/>
-      <c r="B46" s="76"/>
+      <c r="B46" s="83"/>
       <c r="C46" s="6" t="s">
         <v>26</v>
       </c>
@@ -3215,7 +3233,7 @@
     </row>
     <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="53"/>
-      <c r="B47" s="76"/>
+      <c r="B47" s="83"/>
       <c r="C47" s="6" t="s">
         <v>27</v>
       </c>
@@ -3223,7 +3241,7 @@
     </row>
     <row r="48" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="53"/>
-      <c r="B48" s="76"/>
+      <c r="B48" s="83"/>
       <c r="C48" s="6" t="s">
         <v>28</v>
       </c>
@@ -3231,7 +3249,7 @@
     </row>
     <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="53"/>
-      <c r="B49" s="76"/>
+      <c r="B49" s="83"/>
       <c r="C49" s="6" t="s">
         <v>29</v>
       </c>
@@ -3239,7 +3257,7 @@
     </row>
     <row r="50" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="53"/>
-      <c r="B50" s="76"/>
+      <c r="B50" s="83"/>
       <c r="C50" s="6" t="s">
         <v>30</v>
       </c>
@@ -3247,7 +3265,7 @@
     </row>
     <row r="51" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="53"/>
-      <c r="B51" s="76"/>
+      <c r="B51" s="83"/>
       <c r="C51" s="6" t="s">
         <v>31</v>
       </c>
@@ -3255,7 +3273,7 @@
     </row>
     <row r="52" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="53"/>
-      <c r="B52" s="76"/>
+      <c r="B52" s="83"/>
       <c r="C52" s="6" t="s">
         <v>32</v>
       </c>
@@ -3263,7 +3281,7 @@
     </row>
     <row r="53" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="53"/>
-      <c r="B53" s="77"/>
+      <c r="B53" s="84"/>
       <c r="C53" s="6" t="s">
         <v>33</v>
       </c>
@@ -3271,7 +3289,7 @@
     </row>
     <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="53"/>
-      <c r="B54" s="75" t="s">
+      <c r="B54" s="82" t="s">
         <v>34</v>
       </c>
       <c r="C54" s="6" t="s">
@@ -3279,27 +3297,27 @@
       </c>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="53">
         <v>5</v>
       </c>
-      <c r="B55" s="76"/>
+      <c r="B55" s="83"/>
       <c r="C55" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D55" s="4"/>
-    </row>
-    <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D55" s="76"/>
+    </row>
+    <row r="56" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="53"/>
-      <c r="B56" s="76"/>
+      <c r="B56" s="83"/>
       <c r="C56" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D56" s="4"/>
+      <c r="D56" s="76"/>
     </row>
     <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="53"/>
-      <c r="B57" s="76"/>
+      <c r="B57" s="83"/>
       <c r="C57" s="7" t="s">
         <v>14</v>
       </c>
@@ -3307,7 +3325,7 @@
     </row>
     <row r="58" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="53"/>
-      <c r="B58" s="76"/>
+      <c r="B58" s="83"/>
       <c r="C58" s="6" t="s">
         <v>15</v>
       </c>
@@ -3315,7 +3333,7 @@
     </row>
     <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="53"/>
-      <c r="B59" s="76"/>
+      <c r="B59" s="83"/>
       <c r="C59" s="6" t="s">
         <v>16</v>
       </c>
@@ -3323,7 +3341,7 @@
     </row>
     <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="53"/>
-      <c r="B60" s="76"/>
+      <c r="B60" s="83"/>
       <c r="C60" s="6" t="s">
         <v>17</v>
       </c>
@@ -3331,7 +3349,7 @@
     </row>
     <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="53"/>
-      <c r="B61" s="76"/>
+      <c r="B61" s="83"/>
       <c r="C61" s="6" t="s">
         <v>18</v>
       </c>
@@ -3339,23 +3357,25 @@
     </row>
     <row r="62" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="53"/>
-      <c r="B62" s="76"/>
+      <c r="B62" s="83"/>
       <c r="C62" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D62" s="4"/>
     </row>
-    <row r="63" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="53"/>
-      <c r="B63" s="76"/>
+      <c r="B63" s="83"/>
       <c r="C63" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D63" s="4"/>
+      <c r="D63" s="63" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="64" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="53"/>
-      <c r="B64" s="76"/>
+      <c r="B64" s="83"/>
       <c r="C64" s="6" t="s">
         <v>21</v>
       </c>
@@ -3363,17 +3383,15 @@
     </row>
     <row r="65" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="53"/>
-      <c r="B65" s="76"/>
+      <c r="B65" s="83"/>
       <c r="C65" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D65" s="74" t="s">
-        <v>628</v>
-      </c>
+      <c r="D65" s="76"/>
     </row>
     <row r="66" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="53"/>
-      <c r="B66" s="76"/>
+      <c r="B66" s="83"/>
       <c r="C66" s="6" t="s">
         <v>23</v>
       </c>
@@ -3381,7 +3399,7 @@
     </row>
     <row r="67" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="53"/>
-      <c r="B67" s="76"/>
+      <c r="B67" s="83"/>
       <c r="C67" s="6" t="s">
         <v>24</v>
       </c>
@@ -3389,7 +3407,7 @@
     </row>
     <row r="68" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="53"/>
-      <c r="B68" s="76"/>
+      <c r="B68" s="83"/>
       <c r="C68" s="6" t="s">
         <v>25</v>
       </c>
@@ -3397,7 +3415,7 @@
     </row>
     <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="53"/>
-      <c r="B69" s="76"/>
+      <c r="B69" s="83"/>
       <c r="C69" s="6" t="s">
         <v>26</v>
       </c>
@@ -3405,7 +3423,7 @@
     </row>
     <row r="70" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="53"/>
-      <c r="B70" s="76"/>
+      <c r="B70" s="83"/>
       <c r="C70" s="6" t="s">
         <v>27</v>
       </c>
@@ -3413,7 +3431,7 @@
     </row>
     <row r="71" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="53"/>
-      <c r="B71" s="76"/>
+      <c r="B71" s="83"/>
       <c r="C71" s="6" t="s">
         <v>28</v>
       </c>
@@ -3421,7 +3439,7 @@
     </row>
     <row r="72" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="53"/>
-      <c r="B72" s="76"/>
+      <c r="B72" s="83"/>
       <c r="C72" s="6" t="s">
         <v>29</v>
       </c>
@@ -3429,7 +3447,7 @@
     </row>
     <row r="73" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="53"/>
-      <c r="B73" s="76"/>
+      <c r="B73" s="83"/>
       <c r="C73" s="6" t="s">
         <v>30</v>
       </c>
@@ -3437,7 +3455,7 @@
     </row>
     <row r="74" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="53"/>
-      <c r="B74" s="76"/>
+      <c r="B74" s="83"/>
       <c r="C74" s="6" t="s">
         <v>31</v>
       </c>
@@ -3445,7 +3463,7 @@
     </row>
     <row r="75" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="53"/>
-      <c r="B75" s="76"/>
+      <c r="B75" s="83"/>
       <c r="C75" s="6" t="s">
         <v>32</v>
       </c>
@@ -3453,7 +3471,7 @@
     </row>
     <row r="76" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="53"/>
-      <c r="B76" s="77"/>
+      <c r="B76" s="84"/>
       <c r="C76" s="6" t="s">
         <v>33</v>
       </c>
@@ -3461,7 +3479,7 @@
     </row>
     <row r="77" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="53"/>
-      <c r="B77" s="75" t="s">
+      <c r="B77" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C77" s="6" t="s">
@@ -3471,25 +3489,27 @@
     </row>
     <row r="78" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="53"/>
-      <c r="B78" s="76"/>
+      <c r="B78" s="83"/>
       <c r="C78" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D78" s="4"/>
     </row>
-    <row r="79" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="53">
         <v>6</v>
       </c>
-      <c r="B79" s="76"/>
+      <c r="B79" s="83"/>
       <c r="C79" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D79" s="4"/>
+      <c r="D79" s="63" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="80" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="53"/>
-      <c r="B80" s="76"/>
+      <c r="B80" s="83"/>
       <c r="C80" s="7" t="s">
         <v>14</v>
       </c>
@@ -3497,7 +3517,7 @@
     </row>
     <row r="81" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="53"/>
-      <c r="B81" s="76"/>
+      <c r="B81" s="83"/>
       <c r="C81" s="6" t="s">
         <v>15</v>
       </c>
@@ -3505,7 +3525,7 @@
     </row>
     <row r="82" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="53"/>
-      <c r="B82" s="76"/>
+      <c r="B82" s="83"/>
       <c r="C82" s="6" t="s">
         <v>16</v>
       </c>
@@ -3513,7 +3533,7 @@
     </row>
     <row r="83" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="53"/>
-      <c r="B83" s="76"/>
+      <c r="B83" s="83"/>
       <c r="C83" s="6" t="s">
         <v>17</v>
       </c>
@@ -3521,7 +3541,7 @@
     </row>
     <row r="84" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="53"/>
-      <c r="B84" s="76"/>
+      <c r="B84" s="83"/>
       <c r="C84" s="6" t="s">
         <v>18</v>
       </c>
@@ -3529,7 +3549,7 @@
     </row>
     <row r="85" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="53"/>
-      <c r="B85" s="76"/>
+      <c r="B85" s="83"/>
       <c r="C85" s="6" t="s">
         <v>19</v>
       </c>
@@ -3537,17 +3557,15 @@
     </row>
     <row r="86" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="53"/>
-      <c r="B86" s="76"/>
+      <c r="B86" s="83"/>
       <c r="C86" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D86" s="74" t="s">
-        <v>628</v>
-      </c>
+      <c r="D86" s="76"/>
     </row>
     <row r="87" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="53"/>
-      <c r="B87" s="76"/>
+      <c r="B87" s="83"/>
       <c r="C87" s="6" t="s">
         <v>21</v>
       </c>
@@ -3555,7 +3573,7 @@
     </row>
     <row r="88" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="53"/>
-      <c r="B88" s="76"/>
+      <c r="B88" s="83"/>
       <c r="C88" s="6" t="s">
         <v>22</v>
       </c>
@@ -3563,7 +3581,7 @@
     </row>
     <row r="89" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="53"/>
-      <c r="B89" s="76"/>
+      <c r="B89" s="83"/>
       <c r="C89" s="6" t="s">
         <v>23</v>
       </c>
@@ -3571,7 +3589,7 @@
     </row>
     <row r="90" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="53"/>
-      <c r="B90" s="76"/>
+      <c r="B90" s="83"/>
       <c r="C90" s="6" t="s">
         <v>24</v>
       </c>
@@ -3579,7 +3597,7 @@
     </row>
     <row r="91" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="53"/>
-      <c r="B91" s="76"/>
+      <c r="B91" s="83"/>
       <c r="C91" s="6" t="s">
         <v>25</v>
       </c>
@@ -3587,71 +3605,71 @@
     </row>
     <row r="92" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="53"/>
-      <c r="B92" s="76"/>
+      <c r="B92" s="83"/>
       <c r="C92" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D92" s="4"/>
     </row>
     <row r="93" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B93" s="76"/>
+      <c r="B93" s="83"/>
       <c r="C93" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D93" s="4"/>
     </row>
     <row r="94" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B94" s="76"/>
+      <c r="B94" s="83"/>
       <c r="C94" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D94" s="4"/>
     </row>
     <row r="95" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B95" s="76"/>
+      <c r="B95" s="83"/>
       <c r="C95" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D95" s="4"/>
     </row>
     <row r="96" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B96" s="76"/>
+      <c r="B96" s="83"/>
       <c r="C96" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D96" s="4"/>
     </row>
     <row r="97" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B97" s="76"/>
+      <c r="B97" s="83"/>
       <c r="C97" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D97" s="4"/>
     </row>
     <row r="98" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B98" s="76"/>
+      <c r="B98" s="83"/>
       <c r="C98" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D98" s="4"/>
     </row>
     <row r="99" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B99" s="77"/>
+      <c r="B99" s="84"/>
       <c r="C99" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D99" s="4"/>
     </row>
     <row r="100" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B100" s="65"/>
-      <c r="C100" s="66"/>
+      <c r="B100" s="85"/>
+      <c r="C100" s="86"/>
       <c r="D100" s="5"/>
     </row>
     <row r="101" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>7</v>
       </c>
-      <c r="B101" s="75" t="s">
+      <c r="B101" s="82" t="s">
         <v>36</v>
       </c>
       <c r="C101" s="6" t="s">
@@ -3660,37 +3678,35 @@
       <c r="D101" s="4"/>
     </row>
     <row r="102" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B102" s="76"/>
+      <c r="B102" s="83"/>
       <c r="C102" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D102" s="4"/>
     </row>
     <row r="103" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B103" s="76"/>
+      <c r="B103" s="83"/>
       <c r="C103" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D103" s="4"/>
     </row>
     <row r="104" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B104" s="76"/>
+      <c r="B104" s="83"/>
       <c r="C104" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D104" s="74" t="s">
-        <v>628</v>
-      </c>
+      <c r="D104" s="76"/>
     </row>
     <row r="105" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B105" s="77"/>
+      <c r="B105" s="84"/>
       <c r="C105" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D105" s="4"/>
     </row>
     <row r="106" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B106" s="75" t="s">
+      <c r="B106" s="82" t="s">
         <v>42</v>
       </c>
       <c r="C106" s="6" t="s">
@@ -3699,7 +3715,7 @@
       <c r="D106" s="4"/>
     </row>
     <row r="107" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B107" s="76"/>
+      <c r="B107" s="83"/>
       <c r="C107" s="6" t="s">
         <v>38</v>
       </c>
@@ -3709,77 +3725,76 @@
       <c r="A108">
         <v>8</v>
       </c>
-      <c r="B108" s="76"/>
+      <c r="B108" s="83"/>
       <c r="C108" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D108" s="4"/>
     </row>
     <row r="109" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B109" s="76"/>
+      <c r="B109" s="83"/>
       <c r="C109" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D109" s="74" t="s">
-        <v>628</v>
-      </c>
+      <c r="D109" s="76"/>
     </row>
     <row r="110" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B110" s="77"/>
+      <c r="B110" s="84"/>
       <c r="C110" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D110" s="4"/>
     </row>
-    <row r="111" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B111" s="75" t="s">
+    <row r="111" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B111" s="82" t="s">
         <v>43</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D111" s="4"/>
-    </row>
-    <row r="112" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B112" s="76"/>
+      <c r="D111" s="63" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B112" s="83"/>
       <c r="C112" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D112" s="4"/>
-    </row>
-    <row r="113" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D112" s="63" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>9</v>
       </c>
-      <c r="B113" s="76"/>
+      <c r="B113" s="83"/>
       <c r="C113" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D113" s="74" t="s">
-        <v>628</v>
-      </c>
     </row>
     <row r="114" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B114" s="76"/>
+      <c r="B114" s="83"/>
       <c r="C114" s="6" t="s">
         <v>40</v>
       </c>
       <c r="D114" s="4"/>
     </row>
     <row r="115" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B115" s="77"/>
+      <c r="B115" s="84"/>
       <c r="C115" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D115" s="4"/>
     </row>
     <row r="116" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B116" s="63"/>
-      <c r="C116" s="64"/>
+      <c r="B116" s="77"/>
+      <c r="C116" s="78"/>
       <c r="D116" s="5"/>
     </row>
     <row r="117" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B117" s="78" t="s">
+      <c r="B117" s="91" t="s">
         <v>44</v>
       </c>
       <c r="C117" s="6" t="s">
@@ -3788,14 +3803,14 @@
       <c r="D117" s="4"/>
     </row>
     <row r="118" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B118" s="79"/>
+      <c r="B118" s="92"/>
       <c r="C118" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D118" s="4"/>
     </row>
     <row r="119" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B119" s="79"/>
+      <c r="B119" s="92"/>
       <c r="C119" s="6" t="s">
         <v>47</v>
       </c>
@@ -3805,51 +3820,51 @@
       <c r="A120">
         <v>10</v>
       </c>
-      <c r="B120" s="79"/>
+      <c r="B120" s="92"/>
       <c r="C120" s="6" t="s">
         <v>48</v>
       </c>
       <c r="D120" s="4"/>
     </row>
     <row r="121" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B121" s="79"/>
+      <c r="B121" s="92"/>
       <c r="C121" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D121" s="4"/>
     </row>
     <row r="122" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B122" s="79"/>
+      <c r="B122" s="92"/>
       <c r="C122" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D122" s="74" t="s">
+      <c r="D122" s="63" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B123" s="79"/>
+      <c r="B123" s="92"/>
       <c r="C123" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D123" s="4"/>
     </row>
     <row r="124" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B124" s="79"/>
+      <c r="B124" s="92"/>
       <c r="C124" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D124" s="4"/>
     </row>
     <row r="125" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B125" s="80"/>
+      <c r="B125" s="93"/>
       <c r="C125" s="6" t="s">
         <v>53</v>
       </c>
       <c r="D125" s="4"/>
     </row>
     <row r="126" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B126" s="78" t="s">
+      <c r="B126" s="91" t="s">
         <v>54</v>
       </c>
       <c r="C126" s="6" t="s">
@@ -3858,84 +3873,86 @@
       <c r="D126" s="4"/>
     </row>
     <row r="127" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B127" s="79"/>
+      <c r="B127" s="92"/>
       <c r="C127" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D127" s="4"/>
     </row>
     <row r="128" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B128" s="79"/>
+      <c r="B128" s="92"/>
       <c r="C128" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D128" s="4"/>
     </row>
     <row r="129" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B129" s="79"/>
+      <c r="B129" s="92"/>
       <c r="C129" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D129" s="74" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D129" s="76"/>
+    </row>
+    <row r="130" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>11</v>
       </c>
-      <c r="B130" s="79"/>
+      <c r="B130" s="92"/>
       <c r="C130" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D130" s="4"/>
+      <c r="D130" s="63" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="131" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B131" s="79"/>
+      <c r="B131" s="92"/>
       <c r="C131" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D131" s="4"/>
     </row>
     <row r="132" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B132" s="79"/>
+      <c r="B132" s="92"/>
       <c r="C132" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D132" s="4"/>
     </row>
     <row r="133" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B133" s="79"/>
+      <c r="B133" s="92"/>
       <c r="C133" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D133" s="4"/>
     </row>
     <row r="134" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B134" s="80"/>
+      <c r="B134" s="93"/>
       <c r="C134" s="6" t="s">
         <v>53</v>
       </c>
       <c r="D134" s="4"/>
     </row>
-    <row r="135" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B135" s="78" t="s">
+    <row r="135" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B135" s="91" t="s">
         <v>55</v>
       </c>
       <c r="C135" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D135" s="4"/>
+      <c r="D135" s="63" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="136" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B136" s="79"/>
+      <c r="B136" s="92"/>
       <c r="C136" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D136" s="4"/>
     </row>
     <row r="137" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B137" s="79"/>
+      <c r="B137" s="92"/>
       <c r="C137" s="6" t="s">
         <v>47</v>
       </c>
@@ -3945,86 +3962,84 @@
       <c r="A138">
         <v>12</v>
       </c>
-      <c r="B138" s="79"/>
+      <c r="B138" s="92"/>
       <c r="C138" s="6" t="s">
         <v>48</v>
       </c>
       <c r="D138" s="4"/>
     </row>
     <row r="139" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B139" s="79"/>
+      <c r="B139" s="92"/>
       <c r="C139" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D139" s="74" t="s">
-        <v>628</v>
-      </c>
+      <c r="D139" s="76"/>
     </row>
     <row r="140" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B140" s="79"/>
+      <c r="B140" s="92"/>
       <c r="C140" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D140" s="4"/>
     </row>
     <row r="141" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B141" s="79"/>
+      <c r="B141" s="92"/>
       <c r="C141" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D141" s="4"/>
     </row>
     <row r="142" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B142" s="79"/>
+      <c r="B142" s="92"/>
       <c r="C142" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D142" s="4"/>
     </row>
     <row r="143" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B143" s="80"/>
+      <c r="B143" s="93"/>
       <c r="C143" s="6" t="s">
         <v>53</v>
       </c>
       <c r="D143" s="4"/>
     </row>
     <row r="144" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B144" s="65"/>
-      <c r="C144" s="66"/>
+      <c r="B144" s="85"/>
+      <c r="C144" s="86"/>
       <c r="D144" s="5"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B145" s="81" t="s">
+      <c r="B145" s="94" t="s">
         <v>56</v>
       </c>
-      <c r="C145" s="67" t="s">
+      <c r="C145" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="D145" s="69"/>
+      <c r="D145" s="89"/>
     </row>
     <row r="146" spans="1:4" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B146" s="82"/>
-      <c r="C146" s="68"/>
-      <c r="D146" s="70"/>
+      <c r="B146" s="95"/>
+      <c r="C146" s="88"/>
+      <c r="D146" s="90"/>
     </row>
     <row r="147" spans="1:4" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="82"/>
-      <c r="C147" s="67" t="s">
+      <c r="B147" s="95"/>
+      <c r="C147" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="D147" s="69"/>
+      <c r="D147" s="89"/>
     </row>
     <row r="148" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B148" s="82"/>
-      <c r="C148" s="68"/>
-      <c r="D148" s="70"/>
+      <c r="B148" s="95"/>
+      <c r="C148" s="88"/>
+      <c r="D148" s="90"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B149" s="82"/>
-      <c r="C149" s="67" t="s">
+      <c r="B149" s="95"/>
+      <c r="C149" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="D149" s="72" t="s">
+      <c r="D149" s="97" t="s">
         <v>628</v>
       </c>
     </row>
@@ -4032,203 +4047,203 @@
       <c r="A150">
         <v>13</v>
       </c>
-      <c r="B150" s="82"/>
-      <c r="C150" s="68"/>
-      <c r="D150" s="73"/>
+      <c r="B150" s="95"/>
+      <c r="C150" s="88"/>
+      <c r="D150" s="98"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B151" s="82"/>
-      <c r="C151" s="67" t="s">
+      <c r="B151" s="95"/>
+      <c r="C151" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="D151" s="69"/>
+      <c r="D151" s="89"/>
     </row>
     <row r="152" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B152" s="82"/>
-      <c r="C152" s="68"/>
-      <c r="D152" s="70"/>
+      <c r="B152" s="95"/>
+      <c r="C152" s="88"/>
+      <c r="D152" s="90"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B153" s="82"/>
-      <c r="C153" s="67" t="s">
+      <c r="B153" s="95"/>
+      <c r="C153" s="87" t="s">
         <v>61</v>
       </c>
-      <c r="D153" s="69"/>
+      <c r="D153" s="89"/>
     </row>
     <row r="154" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B154" s="82"/>
-      <c r="C154" s="68"/>
-      <c r="D154" s="70"/>
+      <c r="B154" s="95"/>
+      <c r="C154" s="88"/>
+      <c r="D154" s="90"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B155" s="82"/>
-      <c r="C155" s="67" t="s">
+      <c r="B155" s="95"/>
+      <c r="C155" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="D155" s="69"/>
+      <c r="D155" s="89"/>
     </row>
     <row r="156" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B156" s="83"/>
-      <c r="C156" s="68"/>
-      <c r="D156" s="70"/>
+      <c r="B156" s="96"/>
+      <c r="C156" s="88"/>
+      <c r="D156" s="90"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B157" s="81" t="s">
+      <c r="B157" s="94" t="s">
         <v>63</v>
       </c>
-      <c r="C157" s="67" t="s">
+      <c r="C157" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="D157" s="69"/>
+      <c r="D157" s="97" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="158" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B158" s="82"/>
-      <c r="C158" s="68"/>
-      <c r="D158" s="70"/>
+      <c r="B158" s="95"/>
+      <c r="C158" s="88"/>
+      <c r="D158" s="98"/>
     </row>
     <row r="159" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="82"/>
-      <c r="C159" s="67" t="s">
+      <c r="B159" s="95"/>
+      <c r="C159" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="D159" s="72" t="s">
-        <v>628</v>
-      </c>
+      <c r="D159" s="103"/>
     </row>
     <row r="160" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B160" s="82"/>
-      <c r="C160" s="68"/>
-      <c r="D160" s="73"/>
+      <c r="B160" s="95"/>
+      <c r="C160" s="88"/>
+      <c r="D160" s="104"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>14</v>
       </c>
-      <c r="B161" s="82"/>
-      <c r="C161" s="67" t="s">
+      <c r="B161" s="95"/>
+      <c r="C161" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="D161" s="69"/>
+      <c r="D161" s="89"/>
     </row>
     <row r="162" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B162" s="82"/>
-      <c r="C162" s="68"/>
-      <c r="D162" s="70"/>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B163" s="82"/>
-      <c r="C163" s="67" t="s">
+      <c r="B162" s="95"/>
+      <c r="C162" s="88"/>
+      <c r="D162" s="90"/>
+    </row>
+    <row r="163" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B163" s="95"/>
+      <c r="C163" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="D163" s="69"/>
-    </row>
-    <row r="164" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B164" s="82"/>
-      <c r="C164" s="68"/>
-      <c r="D164" s="70"/>
+      <c r="D163" s="97" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B164" s="95"/>
+      <c r="C164" s="88"/>
+      <c r="D164" s="98"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B165" s="82"/>
-      <c r="C165" s="67" t="s">
+      <c r="B165" s="95"/>
+      <c r="C165" s="87" t="s">
         <v>61</v>
       </c>
-      <c r="D165" s="69"/>
+      <c r="D165" s="89"/>
     </row>
     <row r="166" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B166" s="82"/>
-      <c r="C166" s="68"/>
-      <c r="D166" s="70"/>
+      <c r="B166" s="95"/>
+      <c r="C166" s="88"/>
+      <c r="D166" s="90"/>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B167" s="82"/>
-      <c r="C167" s="67" t="s">
+      <c r="B167" s="95"/>
+      <c r="C167" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="D167" s="69"/>
+      <c r="D167" s="89"/>
     </row>
     <row r="168" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B168" s="83"/>
-      <c r="C168" s="68"/>
-      <c r="D168" s="70"/>
+      <c r="B168" s="96"/>
+      <c r="C168" s="88"/>
+      <c r="D168" s="90"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B169" s="81" t="s">
+      <c r="B169" s="94" t="s">
         <v>64</v>
       </c>
-      <c r="C169" s="67" t="s">
+      <c r="C169" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="D169" s="69"/>
+      <c r="D169" s="89"/>
     </row>
     <row r="170" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B170" s="82"/>
-      <c r="C170" s="68"/>
-      <c r="D170" s="70"/>
+      <c r="B170" s="95"/>
+      <c r="C170" s="88"/>
+      <c r="D170" s="90"/>
     </row>
     <row r="171" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B171" s="82"/>
-      <c r="C171" s="67" t="s">
+      <c r="B171" s="95"/>
+      <c r="C171" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="D171" s="72" t="s">
-        <v>628</v>
-      </c>
+      <c r="D171" s="103"/>
     </row>
     <row r="172" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B172" s="82"/>
-      <c r="C172" s="68"/>
-      <c r="D172" s="73"/>
+      <c r="B172" s="95"/>
+      <c r="C172" s="88"/>
+      <c r="D172" s="104"/>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>15</v>
       </c>
-      <c r="B173" s="82"/>
-      <c r="C173" s="67" t="s">
+      <c r="B173" s="95"/>
+      <c r="C173" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="D173" s="69"/>
+      <c r="D173" s="89"/>
     </row>
     <row r="174" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B174" s="82"/>
-      <c r="C174" s="68"/>
-      <c r="D174" s="70"/>
+      <c r="B174" s="95"/>
+      <c r="C174" s="88"/>
+      <c r="D174" s="90"/>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B175" s="82"/>
-      <c r="C175" s="67" t="s">
+      <c r="B175" s="95"/>
+      <c r="C175" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="D175" s="69"/>
+      <c r="D175" s="89"/>
     </row>
     <row r="176" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B176" s="82"/>
-      <c r="C176" s="68"/>
-      <c r="D176" s="70"/>
+      <c r="B176" s="95"/>
+      <c r="C176" s="88"/>
+      <c r="D176" s="90"/>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B177" s="82"/>
-      <c r="C177" s="67" t="s">
+      <c r="B177" s="95"/>
+      <c r="C177" s="87" t="s">
         <v>61</v>
       </c>
-      <c r="D177" s="69"/>
+      <c r="D177" s="89"/>
     </row>
     <row r="178" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B178" s="82"/>
-      <c r="C178" s="68"/>
-      <c r="D178" s="70"/>
+      <c r="B178" s="95"/>
+      <c r="C178" s="88"/>
+      <c r="D178" s="90"/>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B179" s="82"/>
-      <c r="C179" s="67" t="s">
+      <c r="B179" s="95"/>
+      <c r="C179" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="D179" s="69"/>
+      <c r="D179" s="89"/>
     </row>
     <row r="180" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B180" s="83"/>
-      <c r="C180" s="68"/>
-      <c r="D180" s="70"/>
+      <c r="B180" s="96"/>
+      <c r="C180" s="88"/>
+      <c r="D180" s="90"/>
     </row>
     <row r="181" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B181" s="9"/>
@@ -4245,16 +4260,14 @@
       <c r="C182" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D182" s="72" t="s">
-        <v>628</v>
-      </c>
+      <c r="D182" s="103"/>
     </row>
     <row r="183" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B183" s="11"/>
       <c r="C183" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D183" s="73"/>
+      <c r="D183" s="104"/>
     </row>
     <row r="184" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B184" s="11"/>
@@ -4282,30 +4295,30 @@
       <c r="C187" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D187" s="72" t="s">
-        <v>628</v>
-      </c>
+      <c r="D187" s="103"/>
     </row>
     <row r="188" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B188" s="11"/>
       <c r="C188" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D188" s="73"/>
-    </row>
-    <row r="189" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D188" s="104"/>
+    </row>
+    <row r="189" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>17</v>
       </c>
-      <c r="B189" s="84" t="s">
+      <c r="B189" s="64" t="s">
         <v>92</v>
       </c>
       <c r="C189" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D189" s="4"/>
-    </row>
-    <row r="190" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D189" s="63" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B190" s="11"/>
       <c r="C190" s="6" t="s">
         <v>15</v>
@@ -4347,26 +4360,26 @@
       </c>
       <c r="D195" s="4"/>
     </row>
-    <row r="196" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A196">
         <v>18</v>
       </c>
-      <c r="B196" s="84" t="s">
+      <c r="B196" s="64" t="s">
         <v>90</v>
       </c>
       <c r="C196" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D196" s="72" t="s">
+      <c r="D196" s="97" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B197" s="11"/>
       <c r="C197" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D197" s="73"/>
+      <c r="D197" s="98"/>
     </row>
     <row r="198" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B198" s="11"/>
@@ -4401,28 +4414,28 @@
       <c r="C202" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D202" s="72" t="s">
-        <v>628</v>
-      </c>
+      <c r="D202" s="103"/>
     </row>
     <row r="203" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A203">
         <v>19</v>
       </c>
-      <c r="B203" s="84" t="s">
+      <c r="B203" s="64" t="s">
         <v>91</v>
       </c>
       <c r="C203" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D203" s="73"/>
-    </row>
-    <row r="204" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D203" s="104"/>
+    </row>
+    <row r="204" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B204" s="11"/>
       <c r="C204" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D204" s="4"/>
+      <c r="D204" s="63" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="205" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B205" s="11"/>
@@ -4460,8 +4473,8 @@
       <c r="D209" s="4"/>
     </row>
     <row r="210" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B210" s="65"/>
-      <c r="C210" s="66"/>
+      <c r="B210" s="85"/>
+      <c r="C210" s="86"/>
       <c r="D210" s="5"/>
     </row>
     <row r="211" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4475,97 +4488,97 @@
       <c r="A212">
         <v>20</v>
       </c>
-      <c r="B212" s="85" t="s">
+      <c r="B212" s="65" t="s">
         <v>109</v>
       </c>
       <c r="C212" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D212" s="69"/>
+      <c r="D212" s="89"/>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B213" s="13"/>
       <c r="C213" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="D213" s="71"/>
+      <c r="D213" s="99"/>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B214" s="13"/>
       <c r="C214" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="D214" s="71"/>
+      <c r="D214" s="99"/>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B215" s="13"/>
       <c r="C215" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D215" s="71"/>
+      <c r="D215" s="99"/>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B216" s="13"/>
       <c r="C216" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D216" s="71"/>
+      <c r="D216" s="99"/>
     </row>
     <row r="217" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B217" s="13"/>
       <c r="C217" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D217" s="70"/>
+      <c r="D217" s="90"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B218" s="13"/>
       <c r="C218" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="D218" s="69"/>
+      <c r="D218" s="89"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B219" s="13"/>
       <c r="C219" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D219" s="71"/>
+      <c r="D219" s="99"/>
     </row>
     <row r="220" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B220" s="13"/>
       <c r="C220" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D220" s="70"/>
+      <c r="D220" s="90"/>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B221" s="13"/>
       <c r="C221" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D221" s="69"/>
+      <c r="D221" s="89"/>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B222" s="13"/>
       <c r="C222" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="D222" s="71"/>
+      <c r="D222" s="99"/>
     </row>
     <row r="223" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B223" s="13"/>
       <c r="C223" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D223" s="70"/>
+      <c r="D223" s="90"/>
     </row>
     <row r="224" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B224" s="13"/>
       <c r="C224" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="D224" s="72" t="s">
+      <c r="D224" s="97" t="s">
         <v>628</v>
       </c>
     </row>
@@ -4574,7 +4587,7 @@
       <c r="C225" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="D225" s="73"/>
+      <c r="D225" s="98"/>
     </row>
     <row r="226" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B226" s="13"/>
@@ -4616,21 +4629,21 @@
       <c r="C231" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D231" s="69"/>
+      <c r="D231" s="89"/>
     </row>
     <row r="232" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B232" s="13"/>
       <c r="C232" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="D232" s="71"/>
+      <c r="D232" s="99"/>
     </row>
     <row r="233" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B233" s="13"/>
       <c r="C233" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="D233" s="70"/>
+      <c r="D233" s="90"/>
     </row>
     <row r="234" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B234" s="13"/>
@@ -4679,21 +4692,21 @@
       <c r="C240" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D240" s="69"/>
+      <c r="D240" s="89"/>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B241" s="13"/>
       <c r="C241" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D241" s="71"/>
+      <c r="D241" s="99"/>
     </row>
     <row r="242" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B242" s="13"/>
       <c r="C242" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="D242" s="70"/>
+      <c r="D242" s="90"/>
     </row>
     <row r="243" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B243" s="13"/>
@@ -4707,42 +4720,42 @@
       <c r="C244" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="D244" s="69"/>
+      <c r="D244" s="89"/>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B245" s="13"/>
       <c r="C245" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="D245" s="71"/>
+      <c r="D245" s="99"/>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B246" s="13"/>
       <c r="C246" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D246" s="71"/>
+      <c r="D246" s="99"/>
     </row>
     <row r="247" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B247" s="13"/>
       <c r="C247" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="D247" s="70"/>
+      <c r="D247" s="90"/>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B248" s="13"/>
       <c r="C248" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="D248" s="69"/>
+      <c r="D248" s="89"/>
     </row>
     <row r="249" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B249" s="13"/>
       <c r="C249" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D249" s="70"/>
+      <c r="D249" s="90"/>
     </row>
     <row r="250" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B250" s="14"/>
@@ -4760,106 +4773,104 @@
       <c r="A252">
         <v>21</v>
       </c>
-      <c r="B252" s="85" t="s">
+      <c r="B252" s="65" t="s">
         <v>110</v>
       </c>
-      <c r="C252" s="12" t="s">
+      <c r="C252" s="105" t="s">
         <v>72</v>
       </c>
-      <c r="D252" s="69"/>
+      <c r="D252" s="89"/>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B253" s="13"/>
       <c r="C253" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="D253" s="71"/>
+      <c r="D253" s="99"/>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B254" s="13"/>
       <c r="C254" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="D254" s="71"/>
+      <c r="D254" s="99"/>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B255" s="13"/>
       <c r="C255" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D255" s="71"/>
+      <c r="D255" s="99"/>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B256" s="13"/>
       <c r="C256" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D256" s="71"/>
+      <c r="D256" s="99"/>
     </row>
     <row r="257" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B257" s="13"/>
       <c r="C257" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D257" s="70"/>
+      <c r="D257" s="90"/>
     </row>
     <row r="258" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B258" s="13"/>
-      <c r="C258" s="12" t="s">
+      <c r="C258" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="D258" s="69"/>
+      <c r="D258" s="89"/>
     </row>
     <row r="259" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B259" s="13"/>
       <c r="C259" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D259" s="71"/>
+      <c r="D259" s="99"/>
     </row>
     <row r="260" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B260" s="13"/>
       <c r="C260" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D260" s="70"/>
+      <c r="D260" s="90"/>
     </row>
     <row r="261" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B261" s="13"/>
       <c r="C261" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D261" s="69"/>
+      <c r="D261" s="89"/>
     </row>
     <row r="262" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B262" s="13"/>
       <c r="C262" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="D262" s="71"/>
+      <c r="D262" s="99"/>
     </row>
     <row r="263" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B263" s="13"/>
       <c r="C263" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D263" s="70"/>
+      <c r="D263" s="90"/>
     </row>
     <row r="264" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B264" s="13"/>
       <c r="C264" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="D264" s="72" t="s">
-        <v>628</v>
-      </c>
+      <c r="D264" s="103"/>
     </row>
     <row r="265" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B265" s="13"/>
       <c r="C265" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="D265" s="73"/>
+      <c r="D265" s="104"/>
     </row>
     <row r="266" spans="2:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B266" s="13"/>
@@ -4880,21 +4891,21 @@
       <c r="C268" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D268" s="69"/>
+      <c r="D268" s="89"/>
     </row>
     <row r="269" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B269" s="13"/>
       <c r="C269" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="D269" s="71"/>
+      <c r="D269" s="99"/>
     </row>
     <row r="270" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B270" s="13"/>
       <c r="C270" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="D270" s="70"/>
+      <c r="D270" s="90"/>
     </row>
     <row r="271" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B271" s="13"/>
@@ -4936,21 +4947,21 @@
       <c r="C276" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D276" s="69"/>
+      <c r="D276" s="89"/>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B277" s="13"/>
       <c r="C277" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D277" s="71"/>
+      <c r="D277" s="99"/>
     </row>
     <row r="278" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B278" s="13"/>
       <c r="C278" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="D278" s="70"/>
+      <c r="D278" s="90"/>
     </row>
     <row r="279" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B279" s="13"/>
@@ -4964,42 +4975,42 @@
       <c r="C280" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="D280" s="69"/>
+      <c r="D280" s="89"/>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B281" s="13"/>
       <c r="C281" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="D281" s="71"/>
+      <c r="D281" s="99"/>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B282" s="13"/>
       <c r="C282" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D282" s="71"/>
+      <c r="D282" s="99"/>
     </row>
     <row r="283" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B283" s="13"/>
       <c r="C283" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="D283" s="70"/>
+      <c r="D283" s="90"/>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B284" s="13"/>
       <c r="C284" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="D284" s="69"/>
+      <c r="D284" s="89"/>
     </row>
     <row r="285" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B285" s="13"/>
       <c r="C285" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D285" s="70"/>
+      <c r="D285" s="90"/>
     </row>
     <row r="286" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B286" s="14"/>
@@ -5017,106 +5028,104 @@
       <c r="A288">
         <v>22</v>
       </c>
-      <c r="B288" s="85" t="s">
+      <c r="B288" s="65" t="s">
         <v>111</v>
       </c>
       <c r="C288" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D288" s="69"/>
+      <c r="D288" s="89"/>
     </row>
     <row r="289" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B289" s="13"/>
       <c r="C289" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="D289" s="71"/>
+      <c r="D289" s="99"/>
     </row>
     <row r="290" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B290" s="13"/>
       <c r="C290" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="D290" s="71"/>
+      <c r="D290" s="99"/>
     </row>
     <row r="291" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B291" s="13"/>
       <c r="C291" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D291" s="71"/>
+      <c r="D291" s="99"/>
     </row>
     <row r="292" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B292" s="13"/>
       <c r="C292" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D292" s="71"/>
+      <c r="D292" s="99"/>
     </row>
     <row r="293" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B293" s="13"/>
       <c r="C293" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D293" s="70"/>
+      <c r="D293" s="90"/>
     </row>
     <row r="294" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B294" s="13"/>
       <c r="C294" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="D294" s="69"/>
+      <c r="D294" s="89"/>
     </row>
     <row r="295" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B295" s="13"/>
       <c r="C295" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D295" s="71"/>
+      <c r="D295" s="99"/>
     </row>
     <row r="296" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B296" s="13"/>
       <c r="C296" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D296" s="70"/>
+      <c r="D296" s="90"/>
     </row>
     <row r="297" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B297" s="13"/>
       <c r="C297" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D297" s="69"/>
+      <c r="D297" s="89"/>
     </row>
     <row r="298" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B298" s="13"/>
       <c r="C298" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="D298" s="71"/>
+      <c r="D298" s="99"/>
     </row>
     <row r="299" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B299" s="13"/>
       <c r="C299" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D299" s="70"/>
+      <c r="D299" s="90"/>
     </row>
     <row r="300" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B300" s="13"/>
       <c r="C300" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="D300" s="72" t="s">
-        <v>628</v>
-      </c>
+      <c r="D300" s="103"/>
     </row>
     <row r="301" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B301" s="13"/>
       <c r="C301" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="D301" s="73"/>
+      <c r="D301" s="104"/>
     </row>
     <row r="302" spans="2:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B302" s="13"/>
@@ -5137,21 +5146,21 @@
       <c r="C304" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D304" s="69"/>
+      <c r="D304" s="89"/>
     </row>
     <row r="305" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B305" s="13"/>
       <c r="C305" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="D305" s="71"/>
+      <c r="D305" s="99"/>
     </row>
     <row r="306" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B306" s="13"/>
       <c r="C306" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="D306" s="70"/>
+      <c r="D306" s="90"/>
     </row>
     <row r="307" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B307" s="13"/>
@@ -5193,21 +5202,21 @@
       <c r="C312" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D312" s="69"/>
+      <c r="D312" s="89"/>
     </row>
     <row r="313" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B313" s="13"/>
       <c r="C313" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D313" s="71"/>
+      <c r="D313" s="99"/>
     </row>
     <row r="314" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B314" s="13"/>
       <c r="C314" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="D314" s="70"/>
+      <c r="D314" s="90"/>
     </row>
     <row r="315" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B315" s="13"/>
@@ -5221,42 +5230,42 @@
       <c r="C316" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="D316" s="69"/>
+      <c r="D316" s="89"/>
     </row>
     <row r="317" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B317" s="13"/>
       <c r="C317" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="D317" s="71"/>
+      <c r="D317" s="99"/>
     </row>
     <row r="318" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B318" s="13"/>
       <c r="C318" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D318" s="71"/>
+      <c r="D318" s="99"/>
     </row>
     <row r="319" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B319" s="13"/>
       <c r="C319" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="D319" s="70"/>
+      <c r="D319" s="90"/>
     </row>
     <row r="320" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B320" s="13"/>
       <c r="C320" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="D320" s="69"/>
+      <c r="D320" s="89"/>
     </row>
     <row r="321" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B321" s="13"/>
       <c r="C321" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D321" s="70"/>
+      <c r="D321" s="90"/>
     </row>
     <row r="322" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B322" s="14"/>
@@ -5274,95 +5283,95 @@
       <c r="A324">
         <v>23</v>
       </c>
-      <c r="B324" s="86" t="s">
+      <c r="B324" s="66" t="s">
         <v>629</v>
       </c>
       <c r="C324" s="12"/>
-      <c r="D324" s="69"/>
+      <c r="D324" s="89"/>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B325" s="13"/>
       <c r="C325" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="D325" s="71"/>
+      <c r="D325" s="99"/>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B326" s="13"/>
       <c r="C326" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="D326" s="71"/>
+      <c r="D326" s="99"/>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B327" s="13"/>
       <c r="C327" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="D327" s="71"/>
+      <c r="D327" s="99"/>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B328" s="13"/>
       <c r="C328" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D328" s="71"/>
+      <c r="D328" s="99"/>
     </row>
     <row r="329" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B329" s="13"/>
       <c r="C329" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="D329" s="70"/>
+      <c r="D329" s="90"/>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B330" s="13"/>
       <c r="C330" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="D330" s="69"/>
+      <c r="D330" s="89"/>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B331" s="13"/>
       <c r="C331" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="D331" s="71"/>
+      <c r="D331" s="99"/>
     </row>
     <row r="332" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B332" s="13"/>
       <c r="C332" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="D332" s="70"/>
+      <c r="D332" s="90"/>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B333" s="13"/>
       <c r="C333" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D333" s="89"/>
+      <c r="D333" s="100"/>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B334" s="13"/>
       <c r="C334" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="D334" s="90"/>
+      <c r="D334" s="101"/>
     </row>
     <row r="335" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B335" s="13"/>
       <c r="C335" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="D335" s="91"/>
+      <c r="D335" s="102"/>
     </row>
     <row r="336" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B336" s="13"/>
       <c r="C336" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="D336" s="88" t="s">
+      <c r="D336" s="68" t="s">
         <v>630</v>
       </c>
     </row>
@@ -5392,21 +5401,21 @@
       <c r="C340" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D340" s="69"/>
+      <c r="D340" s="89"/>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B341" s="13"/>
       <c r="C341" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="D341" s="71"/>
+      <c r="D341" s="99"/>
     </row>
     <row r="342" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B342" s="13"/>
       <c r="C342" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="D342" s="70"/>
+      <c r="D342" s="90"/>
     </row>
     <row r="343" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B343" s="13"/>
@@ -5433,7 +5442,7 @@
       <c r="A346">
         <v>24</v>
       </c>
-      <c r="B346" s="87" t="s">
+      <c r="B346" s="67" t="s">
         <v>144</v>
       </c>
       <c r="C346" s="20" t="s">
@@ -5446,7 +5455,7 @@
       <c r="C347" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D347" s="92" t="s">
+      <c r="D347" s="69" t="s">
         <v>628</v>
       </c>
     </row>
@@ -5755,7 +5764,7 @@
       <c r="A391">
         <v>25</v>
       </c>
-      <c r="B391" s="93" t="s">
+      <c r="B391" s="70" t="s">
         <v>190</v>
       </c>
       <c r="C391" s="20" t="s">
@@ -5768,7 +5777,7 @@
       <c r="C392" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D392" s="94" t="s">
+      <c r="D392" s="71" t="s">
         <v>631</v>
       </c>
     </row>
@@ -6077,7 +6086,7 @@
       <c r="A436">
         <v>26</v>
       </c>
-      <c r="B436" s="93" t="s">
+      <c r="B436" s="70" t="s">
         <v>191</v>
       </c>
       <c r="C436" s="20" t="s">
@@ -6097,7 +6106,7 @@
       <c r="C438" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="D438" s="94" t="s">
+      <c r="D438" s="71" t="s">
         <v>631</v>
       </c>
     </row>
@@ -6399,7 +6408,7 @@
       <c r="A481">
         <v>27</v>
       </c>
-      <c r="B481" s="87" t="s">
+      <c r="B481" s="67" t="s">
         <v>192</v>
       </c>
       <c r="C481" s="20" t="s">
@@ -6412,7 +6421,7 @@
       <c r="C482" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D482" s="96" t="s">
+      <c r="D482" s="73" t="s">
         <v>628</v>
       </c>
     </row>
@@ -7108,7 +7117,7 @@
       <c r="A569">
         <v>29</v>
       </c>
-      <c r="B569" s="87" t="s">
+      <c r="B569" s="67" t="s">
         <v>576</v>
       </c>
       <c r="C569" s="20" t="s">
@@ -7121,7 +7130,7 @@
       <c r="C570" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D570" s="96" t="s">
+      <c r="D570" s="73" t="s">
         <v>628</v>
       </c>
     </row>
@@ -7422,7 +7431,7 @@
       <c r="A613">
         <v>30</v>
       </c>
-      <c r="B613" s="87" t="s">
+      <c r="B613" s="67" t="s">
         <v>577</v>
       </c>
       <c r="C613" s="20" t="s">
@@ -7435,7 +7444,7 @@
       <c r="C614" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D614" s="95" t="s">
+      <c r="D614" s="72" t="s">
         <v>628</v>
       </c>
     </row>
@@ -9297,7 +9306,7 @@
       <c r="A877">
         <v>36</v>
       </c>
-      <c r="B877" s="87" t="s">
+      <c r="B877" s="67" t="s">
         <v>246</v>
       </c>
       <c r="C877" s="20" t="s">
@@ -9310,7 +9319,7 @@
       <c r="C878" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D878" s="95" t="s">
+      <c r="D878" s="72" t="s">
         <v>628</v>
       </c>
     </row>
@@ -9612,7 +9621,7 @@
       <c r="A921">
         <v>37</v>
       </c>
-      <c r="B921" s="93" t="s">
+      <c r="B921" s="70" t="s">
         <v>247</v>
       </c>
       <c r="C921" s="20" t="s">
@@ -9625,7 +9634,7 @@
       <c r="C922" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D922" s="97" t="s">
+      <c r="D922" s="74" t="s">
         <v>628</v>
       </c>
     </row>
@@ -9927,7 +9936,7 @@
       <c r="A965">
         <v>38</v>
       </c>
-      <c r="B965" s="87" t="s">
+      <c r="B965" s="67" t="s">
         <v>248</v>
       </c>
       <c r="C965" s="20" t="s">
@@ -9940,7 +9949,7 @@
       <c r="C966" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D966" s="95" t="s">
+      <c r="D966" s="72" t="s">
         <v>628</v>
       </c>
     </row>
@@ -10242,7 +10251,7 @@
       <c r="A1009">
         <v>39</v>
       </c>
-      <c r="B1009" s="87" t="s">
+      <c r="B1009" s="67" t="s">
         <v>249</v>
       </c>
       <c r="C1009" s="20" t="s">
@@ -10255,7 +10264,7 @@
       <c r="C1010" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D1010" s="95" t="s">
+      <c r="D1010" s="72" t="s">
         <v>628</v>
       </c>
     </row>
@@ -10557,7 +10566,7 @@
       <c r="A1053">
         <v>40</v>
       </c>
-      <c r="B1053" s="93" t="s">
+      <c r="B1053" s="70" t="s">
         <v>250</v>
       </c>
       <c r="C1053" s="20" t="s">
@@ -10570,7 +10579,7 @@
       <c r="C1054" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D1054" s="94" t="s">
+      <c r="D1054" s="71" t="s">
         <v>632</v>
       </c>
     </row>
@@ -10872,7 +10881,7 @@
       <c r="A1097">
         <v>41</v>
       </c>
-      <c r="B1097" s="93" t="s">
+      <c r="B1097" s="70" t="s">
         <v>251</v>
       </c>
       <c r="C1097" s="20" t="s">
@@ -10890,7 +10899,7 @@
       <c r="C1098" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D1098" s="97" t="s">
+      <c r="D1098" s="74" t="s">
         <v>632</v>
       </c>
     </row>
@@ -11219,7 +11228,7 @@
       <c r="A1144">
         <v>45</v>
       </c>
-      <c r="B1144" s="98" t="s">
+      <c r="B1144" s="75" t="s">
         <v>484</v>
       </c>
       <c r="C1144" s="20" t="s">
@@ -15086,11 +15095,12 @@
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="D187:D188"/>
     <mergeCell ref="D196:D197"/>
     <mergeCell ref="D182:D183"/>
     <mergeCell ref="D202:D203"/>
     <mergeCell ref="D224:D225"/>
+    <mergeCell ref="D221:D223"/>
+    <mergeCell ref="D218:D220"/>
     <mergeCell ref="D320:D321"/>
     <mergeCell ref="D324:D329"/>
     <mergeCell ref="D330:D332"/>
@@ -15110,7 +15120,6 @@
     <mergeCell ref="D312:D314"/>
     <mergeCell ref="D264:D265"/>
     <mergeCell ref="D300:D301"/>
-    <mergeCell ref="D221:D223"/>
     <mergeCell ref="D231:D233"/>
     <mergeCell ref="D240:D242"/>
     <mergeCell ref="D244:D247"/>
@@ -15121,7 +15130,6 @@
     <mergeCell ref="D179:D180"/>
     <mergeCell ref="B210:C210"/>
     <mergeCell ref="D212:D217"/>
-    <mergeCell ref="D218:D220"/>
     <mergeCell ref="B169:B180"/>
     <mergeCell ref="C169:C170"/>
     <mergeCell ref="D169:D170"/>
@@ -15132,12 +15140,7 @@
     <mergeCell ref="C175:C176"/>
     <mergeCell ref="D175:D176"/>
     <mergeCell ref="C177:C178"/>
-    <mergeCell ref="C163:C164"/>
-    <mergeCell ref="D163:D164"/>
-    <mergeCell ref="C165:C166"/>
-    <mergeCell ref="D165:D166"/>
-    <mergeCell ref="C167:C168"/>
-    <mergeCell ref="D167:D168"/>
+    <mergeCell ref="D187:D188"/>
     <mergeCell ref="D155:D156"/>
     <mergeCell ref="B157:B168"/>
     <mergeCell ref="C157:C158"/>
@@ -15146,6 +15149,12 @@
     <mergeCell ref="D159:D160"/>
     <mergeCell ref="C161:C162"/>
     <mergeCell ref="D161:D162"/>
+    <mergeCell ref="C163:C164"/>
+    <mergeCell ref="D163:D164"/>
+    <mergeCell ref="C165:C166"/>
+    <mergeCell ref="D165:D166"/>
+    <mergeCell ref="C167:C168"/>
+    <mergeCell ref="D167:D168"/>
     <mergeCell ref="C151:C152"/>
     <mergeCell ref="D151:D152"/>
     <mergeCell ref="B117:B125"/>

</xml_diff>